<commit_message>
late at night. Me is tired. but most of the pathConstructor setup is done. Now need to actually implement search alg.
</commit_message>
<xml_diff>
--- a/placeAttributes.xlsx
+++ b/placeAttributes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="24660" windowHeight="9900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16575" windowHeight="9900"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="274">
   <si>
     <t>360 Gourmet Burritos</t>
   </si>
@@ -65,7 +65,7 @@
     <t>Au Bon Pain, Deli</t>
   </si>
   <si>
-    <t>Low</t>
+    <t>Salad, Bakeries, Sandwiches</t>
   </si>
   <si>
     <t>5:30 - 22:00</t>
@@ -107,9 +107,6 @@
     <t>CRÚ - Food &amp; Wine Bar</t>
   </si>
   <si>
-    <t>Wine Bars</t>
-  </si>
-  <si>
     <t>6:00 - 22:00</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
     <t>Fuddruckers Hamburgers</t>
   </si>
   <si>
+    <t>Burgers, American</t>
+  </si>
+  <si>
     <t>8:30 - 21:00</t>
   </si>
   <si>
@@ -158,6 +158,9 @@
     <t>D31</t>
   </si>
   <si>
+    <t>Sports Bars, American</t>
+  </si>
+  <si>
     <t>6:30 - 22:00</t>
   </si>
   <si>
@@ -173,6 +176,9 @@
     <t>III Forks Prime Steakhouse</t>
   </si>
   <si>
+    <t>Steakhouse</t>
+  </si>
+  <si>
     <t>6:00 - 9:00</t>
   </si>
   <si>
@@ -188,6 +194,9 @@
     <t>D33</t>
   </si>
   <si>
+    <t>Fast Food, Burgers</t>
+  </si>
+  <si>
     <t>4:00 - 22:00</t>
   </si>
   <si>
@@ -209,6 +218,9 @@
     <t>Reata Grill</t>
   </si>
   <si>
+    <t>Tex-Mex, American</t>
+  </si>
+  <si>
     <t>7:00 - 21:00</t>
   </si>
   <si>
@@ -218,6 +230,9 @@
     <t>D17</t>
   </si>
   <si>
+    <t>Latin American, Mexican, Tex-Mex</t>
+  </si>
+  <si>
     <t>11:00 - 22:00</t>
   </si>
   <si>
@@ -233,27 +248,27 @@
     <t>Stampede 66 Express by Stephan Pyles</t>
   </si>
   <si>
+    <t>American, Southwestern</t>
+  </si>
+  <si>
     <t>11:30 - 14:00, 17:00 - 22:00</t>
   </si>
   <si>
     <t>Starbucks Coffee</t>
   </si>
   <si>
-    <t xml:space="preserve"> D25</t>
-  </si>
-  <si>
     <t>5:00 - 21:00</t>
   </si>
   <si>
-    <t xml:space="preserve"> D28</t>
-  </si>
-  <si>
     <t xml:space="preserve"> D30</t>
   </si>
   <si>
     <t>The Italian Kitchen by Wolfgang Puck</t>
   </si>
   <si>
+    <t>Pizza, Italian, Sandwiches</t>
+  </si>
+  <si>
     <t>5:00 -23:00</t>
   </si>
   <si>
@@ -263,9 +278,15 @@
     <t>D20</t>
   </si>
   <si>
+    <t>Irish, Irish Pub</t>
+  </si>
+  <si>
     <t>Whitetail Bistro by Kent Rathbun</t>
   </si>
   <si>
+    <t>French, Diners</t>
+  </si>
+  <si>
     <t>Blimpie</t>
   </si>
   <si>
@@ -275,6 +296,9 @@
     <t>E21</t>
   </si>
   <si>
+    <t>Sandwiches, Fast Food</t>
+  </si>
+  <si>
     <t>10:30 - 20:00</t>
   </si>
   <si>
@@ -296,6 +320,9 @@
     <t>E26</t>
   </si>
   <si>
+    <t>Delis</t>
+  </si>
+  <si>
     <t>Camille's Ice Cream Bars</t>
   </si>
   <si>
@@ -347,6 +374,9 @@
     <t>E11</t>
   </si>
   <si>
+    <t>Burgers, Sandwiches</t>
+  </si>
+  <si>
     <t>11:00 - 20:00</t>
   </si>
   <si>
@@ -395,6 +425,9 @@
     <t>Wendy's</t>
   </si>
   <si>
+    <t>Burgers, Fast Food</t>
+  </si>
+  <si>
     <t>7-Eleven</t>
   </si>
   <si>
@@ -488,9 +521,6 @@
     <t>10:00 - 21:02</t>
   </si>
   <si>
-    <t xml:space="preserve"> Int</t>
-  </si>
-  <si>
     <t>10:00 - 21:03</t>
   </si>
   <si>
@@ -566,9 +596,6 @@
     <t>Luggage Cart</t>
   </si>
   <si>
-    <t>Throughout</t>
-  </si>
-  <si>
     <t>Michael Kors</t>
   </si>
   <si>
@@ -743,6 +770,9 @@
     <t>priceRange</t>
   </si>
   <si>
+    <t>userPreference</t>
+  </si>
+  <si>
     <t>water</t>
   </si>
   <si>
@@ -776,55 +806,49 @@
     <t>placeName</t>
   </si>
   <si>
+    <t>Tapas, Small Plates, Coffee &amp; Tea, Wine Bars</t>
+  </si>
+  <si>
+    <t>Breakfast and Brunch, Soup, Sandwiches</t>
+  </si>
+  <si>
     <t>Ice Cream and Frozen Yogurt</t>
   </si>
   <si>
+    <t>Mexican, Diners, Breafast and Brunch</t>
+  </si>
+  <si>
     <t>Breakfast and Brunch</t>
   </si>
   <si>
     <t>Coffee and Tea</t>
   </si>
   <si>
+    <t>Pizza, Beer, Wine and Spirits, Italian</t>
+  </si>
+  <si>
     <t>Leather Goods</t>
   </si>
   <si>
+    <t>Breakfast and Brunch, Fast Food</t>
+  </si>
+  <si>
+    <t>American, Bars, Breakfast and Brunch</t>
+  </si>
+  <si>
+    <t>Juice Bars and Smoothies, cafes</t>
+  </si>
+  <si>
     <t>Consumables</t>
   </si>
   <si>
     <t>onlineRating</t>
   </si>
   <si>
-    <t>Sandwiches</t>
-  </si>
-  <si>
-    <t>Burgers</t>
-  </si>
-  <si>
-    <t>Cafes</t>
-  </si>
-  <si>
-    <t>French</t>
-  </si>
-  <si>
-    <t>Irish</t>
-  </si>
-  <si>
-    <t>Italian</t>
-  </si>
-  <si>
-    <t>Bakeries</t>
-  </si>
-  <si>
-    <t>Tapas, Small Plates</t>
-  </si>
-  <si>
-    <t>Tex-Mex</t>
-  </si>
-  <si>
-    <t>Mexican, Tex-Mex</t>
-  </si>
-  <si>
-    <t>userRating</t>
+    <t>Wine Bars, Italian</t>
+  </si>
+  <si>
+    <t>D30</t>
   </si>
 </sst>
 </file>
@@ -1186,15 +1210,15 @@
   <dimension ref="A1:U203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="K1" sqref="K1"/>
+      <selection pane="bottomRight" activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
@@ -1217,64 +1241,64 @@
   <sheetData>
     <row r="1" spans="1:21" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>248</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="K1" s="5" t="s">
+      <c r="O1" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="T1" s="5" t="s">
         <v>254</v>
       </c>
-      <c r="L1" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="O1" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>241</v>
-      </c>
-      <c r="R1" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="S1" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="T1" s="5" t="s">
-        <v>244</v>
-      </c>
       <c r="U1" s="8" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1362,13 +1386,13 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H3">
         <v>-1</v>
       </c>
       <c r="I3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J3" t="s">
         <v>7</v>
@@ -1433,7 +1457,7 @@
         <v>-1</v>
       </c>
       <c r="I4" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -1485,8 +1509,8 @@
       <c r="D5" t="s">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>12</v>
+      <c r="E5">
+        <v>-1</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1498,7 +1522,7 @@
         <v>-1</v>
       </c>
       <c r="I5" t="s">
-        <v>261</v>
+        <v>12</v>
       </c>
       <c r="J5" t="s">
         <v>13</v>
@@ -1758,7 +1782,7 @@
         <v>-1</v>
       </c>
       <c r="I9" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="J9" t="s">
         <v>24</v>
@@ -1817,16 +1841,16 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10">
         <v>-1</v>
       </c>
       <c r="I10" t="s">
+        <v>272</v>
+      </c>
+      <c r="J10" t="s">
         <v>26</v>
-      </c>
-      <c r="J10" t="s">
-        <v>27</v>
       </c>
       <c r="K10">
         <v>3.5</v>
@@ -1870,13 +1894,13 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>28</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>29</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1888,7 +1912,7 @@
         <v>-1</v>
       </c>
       <c r="I11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J11" t="s">
         <v>7</v>
@@ -1935,13 +1959,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>31</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>32</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1953,10 +1977,10 @@
         <v>-1</v>
       </c>
       <c r="I12" t="s">
-        <v>3</v>
+        <v>262</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K12">
         <v>3</v>
@@ -2000,13 +2024,13 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>34</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>35</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2018,7 +2042,7 @@
         <v>-1</v>
       </c>
       <c r="I13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J13" t="s">
         <v>7</v>
@@ -2065,7 +2089,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -2083,10 +2107,10 @@
         <v>-1</v>
       </c>
       <c r="I14" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="J14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K14">
         <v>2.5</v>
@@ -2130,7 +2154,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -2148,7 +2172,7 @@
         <v>-1</v>
       </c>
       <c r="I15" t="s">
-        <v>256</v>
+        <v>39</v>
       </c>
       <c r="J15" t="s">
         <v>40</v>
@@ -2213,10 +2237,10 @@
         <v>-1</v>
       </c>
       <c r="I16" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K16">
         <v>4</v>
@@ -2260,13 +2284,13 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2278,10 +2302,10 @@
         <v>-1</v>
       </c>
       <c r="I17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K17">
         <v>4</v>
@@ -2325,7 +2349,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -2337,16 +2361,16 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H18">
         <v>-1</v>
       </c>
       <c r="I18" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="J18" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K18">
         <v>2.5</v>
@@ -2390,13 +2414,13 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F19">
         <v>1</v>
@@ -2408,7 +2432,7 @@
         <v>-1</v>
       </c>
       <c r="I19" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J19" t="s">
         <v>7</v>
@@ -2455,13 +2479,13 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2473,10 +2497,10 @@
         <v>-1</v>
       </c>
       <c r="I20" t="s">
-        <v>256</v>
+        <v>55</v>
       </c>
       <c r="J20" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K20">
         <v>3</v>
@@ -2520,13 +2544,13 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F21">
         <v>1</v>
@@ -2538,10 +2562,10 @@
         <v>-1</v>
       </c>
       <c r="I21" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J21" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="K21">
         <v>3</v>
@@ -2585,7 +2609,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -2603,7 +2627,7 @@
         <v>-1</v>
       </c>
       <c r="I22" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="J22" t="s">
         <v>7</v>
@@ -2650,7 +2674,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -2668,10 +2692,10 @@
         <v>-1</v>
       </c>
       <c r="I23" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K23">
         <v>4</v>
@@ -2715,13 +2739,13 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -2733,10 +2757,10 @@
         <v>-1</v>
       </c>
       <c r="I24" t="s">
-        <v>263</v>
+        <v>63</v>
       </c>
       <c r="J24" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K24">
         <v>3</v>
@@ -2780,13 +2804,13 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2798,10 +2822,10 @@
         <v>-1</v>
       </c>
       <c r="I25" t="s">
-        <v>264</v>
+        <v>67</v>
       </c>
       <c r="J25" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="K25">
         <v>3</v>
@@ -2845,28 +2869,28 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F26">
         <v>1</v>
       </c>
       <c r="G26">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H26">
         <v>-1</v>
       </c>
       <c r="I26" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="J26" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="K26">
         <v>3</v>
@@ -2910,7 +2934,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
@@ -2922,16 +2946,16 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H27">
         <v>-1</v>
       </c>
       <c r="I27" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="J27" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="K27">
         <v>2</v>
@@ -2975,13 +2999,13 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
+        <v>34</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2993,10 +3017,10 @@
         <v>-1</v>
       </c>
       <c r="I28" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J28" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="K28">
         <v>2.5</v>
@@ -3040,13 +3064,13 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>72</v>
+        <v>196</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -3058,10 +3082,10 @@
         <v>-1</v>
       </c>
       <c r="I29" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J29" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="K29">
         <v>2.5</v>
@@ -3105,13 +3129,13 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>73</v>
+        <v>273</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -3123,10 +3147,10 @@
         <v>-1</v>
       </c>
       <c r="I30" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J30" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="K30">
         <v>2.5</v>
@@ -3170,7 +3194,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
@@ -3188,10 +3212,10 @@
         <v>-1</v>
       </c>
       <c r="I31" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J31" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="K31">
         <v>2.5</v>
@@ -3235,28 +3259,28 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F32">
         <v>1</v>
       </c>
       <c r="G32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H32">
         <v>-1</v>
       </c>
       <c r="I32" t="s">
-        <v>260</v>
+        <v>79</v>
       </c>
       <c r="J32" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="K32">
         <v>3.5</v>
@@ -3300,13 +3324,13 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -3318,10 +3342,10 @@
         <v>-1</v>
       </c>
       <c r="I33" t="s">
-        <v>259</v>
+        <v>83</v>
       </c>
       <c r="J33" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="K33">
         <v>3.5</v>
@@ -3365,7 +3389,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -3377,13 +3401,13 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H34">
         <v>-1</v>
       </c>
       <c r="I34" t="s">
-        <v>258</v>
+        <v>85</v>
       </c>
       <c r="J34" t="s">
         <v>7</v>
@@ -3430,13 +3454,13 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="D35" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -3448,10 +3472,10 @@
         <v>-1</v>
       </c>
       <c r="I35" t="s">
-        <v>255</v>
+        <v>89</v>
       </c>
       <c r="J35" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="K35">
         <v>1.5</v>
@@ -3495,13 +3519,13 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="D36" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -3513,10 +3537,10 @@
         <v>-1</v>
       </c>
       <c r="I36" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="J36" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="K36">
         <v>3.5</v>
@@ -3560,13 +3584,13 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" t="s">
         <v>87</v>
       </c>
-      <c r="D37" t="s">
-        <v>80</v>
-      </c>
       <c r="E37" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -3578,7 +3602,7 @@
         <v>-1</v>
       </c>
       <c r="I37" t="s">
-        <v>255</v>
+        <v>97</v>
       </c>
       <c r="J37" t="s">
         <v>7</v>
@@ -3625,13 +3649,13 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E38" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -3643,10 +3667,10 @@
         <v>-1</v>
       </c>
       <c r="I38" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="J38" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="K38">
         <v>4</v>
@@ -3690,13 +3714,13 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D39" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E39" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -3708,7 +3732,7 @@
         <v>-1</v>
       </c>
       <c r="I39" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="J39" t="s">
         <v>10</v>
@@ -3755,13 +3779,13 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D40" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E40" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -3773,10 +3797,10 @@
         <v>-1</v>
       </c>
       <c r="I40" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J40" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K40">
         <v>3</v>
@@ -3820,13 +3844,13 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D41" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E41" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -3838,10 +3862,10 @@
         <v>-1</v>
       </c>
       <c r="I41" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="J41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K41">
         <v>2.5</v>
@@ -3885,13 +3909,13 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="D42" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E42" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -3903,7 +3927,7 @@
         <v>-1</v>
       </c>
       <c r="I42" t="s">
-        <v>36</v>
+        <v>268</v>
       </c>
       <c r="J42" t="s">
         <v>7</v>
@@ -3950,14 +3974,14 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
+        <v>105</v>
+      </c>
+      <c r="D43" t="s">
+        <v>87</v>
+      </c>
+      <c r="E43" t="s">
         <v>96</v>
       </c>
-      <c r="D43" t="s">
-        <v>80</v>
-      </c>
-      <c r="E43" t="s">
-        <v>88</v>
-      </c>
       <c r="F43">
         <v>1</v>
       </c>
@@ -3968,10 +3992,10 @@
         <v>-1</v>
       </c>
       <c r="I43" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="J43" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="K43">
         <v>3</v>
@@ -4015,13 +4039,13 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="D44" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E44" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -4033,10 +4057,10 @@
         <v>-1</v>
       </c>
       <c r="I44" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="J44" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -4080,13 +4104,13 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="D45" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E45" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -4098,10 +4122,10 @@
         <v>-1</v>
       </c>
       <c r="I45" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J45" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="K45">
         <v>2.5</v>
@@ -4145,13 +4169,13 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="D46" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E46" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -4163,10 +4187,10 @@
         <v>-1</v>
       </c>
       <c r="I46" t="s">
-        <v>256</v>
+        <v>115</v>
       </c>
       <c r="J46" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="K46">
         <v>3.5</v>
@@ -4210,13 +4234,13 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="D47" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E47" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -4228,7 +4252,7 @@
         <v>-1</v>
       </c>
       <c r="I47" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J47" t="s">
         <v>7</v>
@@ -4275,13 +4299,13 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D48" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E48" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -4293,10 +4317,10 @@
         <v>-1</v>
       </c>
       <c r="I48" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J48" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="K48">
         <v>2</v>
@@ -4340,13 +4364,13 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="D49" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E49" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -4358,10 +4382,10 @@
         <v>-1</v>
       </c>
       <c r="I49" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="J49" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="K49">
         <v>3.5</v>
@@ -4405,13 +4429,13 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D50" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E50" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -4423,10 +4447,10 @@
         <v>-1</v>
       </c>
       <c r="I50" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J50" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="K50">
         <v>2.5</v>
@@ -4470,13 +4494,13 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="D51" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E51" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -4488,10 +4512,10 @@
         <v>-1</v>
       </c>
       <c r="I51" t="s">
-        <v>251</v>
+        <v>264</v>
       </c>
       <c r="J51" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="K51">
         <v>2.5</v>
@@ -4535,13 +4559,13 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="D52" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E52" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -4553,10 +4577,10 @@
         <v>-1</v>
       </c>
       <c r="I52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J52" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="K52">
         <v>3.5</v>
@@ -4600,13 +4624,13 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>118</v>
+        <v>128</v>
       </c>
       <c r="D53" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E53" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -4618,10 +4642,10 @@
         <v>-1</v>
       </c>
       <c r="I53" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="J53" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="K53">
         <v>2.5</v>
@@ -4665,13 +4689,13 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="D54" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E54" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -4683,7 +4707,7 @@
         <v>-1</v>
       </c>
       <c r="I54" t="s">
-        <v>256</v>
+        <v>132</v>
       </c>
       <c r="J54" t="s">
         <v>10</v>
@@ -4730,13 +4754,13 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F55">
         <v>2</v>
@@ -4745,13 +4769,13 @@
         <v>5</v>
       </c>
       <c r="H55" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="I55">
         <v>-1</v>
       </c>
       <c r="J55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K55">
         <v>-1</v>
@@ -4795,13 +4819,13 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F56">
         <v>2</v>
@@ -4810,13 +4834,13 @@
         <v>12</v>
       </c>
       <c r="H56" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I56">
         <v>-1</v>
       </c>
       <c r="J56" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K56">
         <v>-1</v>
@@ -4860,7 +4884,7 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
@@ -4875,13 +4899,13 @@
         <v>11</v>
       </c>
       <c r="H57" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I57">
         <v>-1</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K57">
         <v>-1</v>
@@ -4925,13 +4949,13 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="F58">
         <v>3</v>
@@ -4940,13 +4964,13 @@
         <v>11</v>
       </c>
       <c r="H58" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I58">
         <v>-1</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K58">
         <v>-1</v>
@@ -4990,13 +5014,13 @@
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F59">
         <v>3</v>
@@ -5005,13 +5029,13 @@
         <v>11</v>
       </c>
       <c r="H59" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I59">
         <v>-1</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K59">
         <v>-1</v>
@@ -5055,13 +5079,13 @@
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -5070,13 +5094,13 @@
         <v>7</v>
       </c>
       <c r="H60" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="I60">
         <v>-1</v>
       </c>
       <c r="J60" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K60">
         <v>3</v>
@@ -5120,13 +5144,13 @@
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -5135,13 +5159,13 @@
         <v>7</v>
       </c>
       <c r="H61" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="I61">
         <v>-1</v>
       </c>
       <c r="J61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K61">
         <v>3</v>
@@ -5185,13 +5209,13 @@
         <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -5200,13 +5224,13 @@
         <v>7</v>
       </c>
       <c r="H62" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="I62">
         <v>-1</v>
       </c>
       <c r="J62" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
       <c r="K62">
         <v>4.5</v>
@@ -5250,13 +5274,13 @@
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>137</v>
+        <v>148</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -5265,13 +5289,13 @@
         <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I63">
         <v>-1</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -5315,13 +5339,13 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D64" t="s">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>139</v>
+        <v>150</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -5330,13 +5354,13 @@
         <v>6</v>
       </c>
       <c r="H64" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I64">
         <v>-1</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -5380,7 +5404,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
@@ -5395,13 +5419,13 @@
         <v>6</v>
       </c>
       <c r="H65" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I65">
         <v>-1</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -5445,13 +5469,13 @@
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>140</v>
+        <v>151</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F66">
         <v>2</v>
@@ -5460,13 +5484,13 @@
         <v>12</v>
       </c>
       <c r="H66" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I66">
         <v>-1</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K66">
         <v>-1</v>
@@ -5510,13 +5534,13 @@
         <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="D67" t="s">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -5525,13 +5549,13 @@
         <v>7</v>
       </c>
       <c r="H67" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="I67">
         <v>-1</v>
       </c>
       <c r="J67" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="K67">
         <v>4</v>
@@ -5575,22 +5599,22 @@
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="D68" t="s">
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="F68">
         <v>2</v>
       </c>
       <c r="G68">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H68" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I68">
         <v>-1</v>
@@ -5640,13 +5664,13 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D69" t="s">
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>148</v>
+        <v>159</v>
       </c>
       <c r="F69">
         <v>2</v>
@@ -5655,7 +5679,7 @@
         <v>9</v>
       </c>
       <c r="H69" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="I69">
         <v>-1</v>
@@ -5705,13 +5729,13 @@
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D70" t="s">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F70">
         <v>2</v>
@@ -5720,13 +5744,13 @@
         <v>9</v>
       </c>
       <c r="H70" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I70">
         <v>-1</v>
       </c>
       <c r="J70" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
       <c r="K70">
         <v>-1</v>
@@ -5770,7 +5794,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
@@ -5785,13 +5809,13 @@
         <v>9</v>
       </c>
       <c r="H71" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I71">
         <v>-1</v>
       </c>
       <c r="J71" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="K71">
         <v>-1</v>
@@ -5835,13 +5859,13 @@
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D72" t="s">
         <v>1</v>
       </c>
-      <c r="E72" t="s">
-        <v>153</v>
+      <c r="E72">
+        <v>-1</v>
       </c>
       <c r="F72">
         <v>2</v>
@@ -5850,13 +5874,13 @@
         <v>9</v>
       </c>
       <c r="H72" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I72">
         <v>-1</v>
       </c>
       <c r="J72" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="K72">
         <v>-1</v>
@@ -5900,13 +5924,13 @@
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D73" t="s">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F73">
         <v>2</v>
@@ -5915,13 +5939,13 @@
         <v>9</v>
       </c>
       <c r="H73" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I73">
         <v>-1</v>
       </c>
       <c r="J73" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="K73">
         <v>-1</v>
@@ -5965,13 +5989,13 @@
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="D74" t="s">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F74">
         <v>2</v>
@@ -5980,13 +6004,13 @@
         <v>18</v>
       </c>
       <c r="H74" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I74">
         <v>-1</v>
       </c>
       <c r="J74" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K74">
         <v>-1</v>
@@ -6030,7 +6054,7 @@
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D75" t="s">
         <v>1</v>
@@ -6039,13 +6063,13 @@
         <v>20</v>
       </c>
       <c r="F75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G75">
         <v>6</v>
       </c>
       <c r="H75" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="I75">
         <v>-1</v>
@@ -6095,13 +6119,13 @@
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D76" t="s">
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -6110,7 +6134,7 @@
         <v>7</v>
       </c>
       <c r="H76" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="I76">
         <v>-1</v>
@@ -6160,13 +6184,13 @@
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="D77" t="s">
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -6175,7 +6199,7 @@
         <v>7</v>
       </c>
       <c r="H77" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="I77">
         <v>-1</v>
@@ -6225,13 +6249,13 @@
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D78" t="s">
         <v>1</v>
       </c>
       <c r="E78" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -6240,13 +6264,13 @@
         <v>2</v>
       </c>
       <c r="H78" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="I78">
         <v>-1</v>
       </c>
       <c r="J78" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="K78">
         <v>4.5</v>
@@ -6290,13 +6314,13 @@
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="D79" t="s">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -6305,13 +6329,13 @@
         <v>7</v>
       </c>
       <c r="H79" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="I79">
         <v>-1</v>
       </c>
       <c r="J79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K79">
         <v>5</v>
@@ -6355,7 +6379,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D80" t="s">
         <v>1</v>
@@ -6370,13 +6394,13 @@
         <v>5</v>
       </c>
       <c r="H80" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I80">
         <v>-1</v>
       </c>
       <c r="J80" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K80">
         <v>-1</v>
@@ -6420,13 +6444,13 @@
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="D81" t="s">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -6435,13 +6459,13 @@
         <v>7</v>
       </c>
       <c r="H81" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="I81">
         <v>-1</v>
       </c>
       <c r="J81" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K81">
         <v>3.5</v>
@@ -6485,7 +6509,7 @@
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D82" t="s">
         <v>1</v>
@@ -6500,13 +6524,13 @@
         <v>6</v>
       </c>
       <c r="H82" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I82">
         <v>-1</v>
       </c>
       <c r="J82" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="K82">
         <v>3</v>
@@ -6550,13 +6574,13 @@
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F83">
         <v>1</v>
@@ -6565,13 +6589,13 @@
         <v>7</v>
       </c>
       <c r="H83" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="I83">
         <v>-1</v>
       </c>
       <c r="J83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K83">
         <v>3.5</v>
@@ -6615,13 +6639,13 @@
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="D84" t="s">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -6630,13 +6654,13 @@
         <v>7</v>
       </c>
       <c r="H84" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="I84">
         <v>-1</v>
       </c>
       <c r="J84" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K84">
         <v>3.5</v>
@@ -6680,7 +6704,7 @@
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="D85" t="s">
         <v>1</v>
@@ -6695,13 +6719,13 @@
         <v>7</v>
       </c>
       <c r="H85" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="I85">
         <v>-1</v>
       </c>
       <c r="J85" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K85">
         <v>3.5</v>
@@ -6745,13 +6769,13 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D86" t="s">
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -6760,7 +6784,7 @@
         <v>6</v>
       </c>
       <c r="H86" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I86">
         <v>-1</v>
@@ -6810,13 +6834,13 @@
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>172</v>
+        <v>182</v>
       </c>
       <c r="D87" t="s">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -6825,13 +6849,13 @@
         <v>12</v>
       </c>
       <c r="H87" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I87">
         <v>-1</v>
       </c>
       <c r="J87" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="K87">
         <v>2.5</v>
@@ -6875,13 +6899,13 @@
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>173</v>
+        <v>183</v>
       </c>
       <c r="D88" t="s">
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -6890,7 +6914,7 @@
         <v>7</v>
       </c>
       <c r="H88" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="I88">
         <v>-1</v>
@@ -6940,7 +6964,7 @@
         <v>87</v>
       </c>
       <c r="C89" t="s">
-        <v>174</v>
+        <v>184</v>
       </c>
       <c r="D89" t="s">
         <v>1</v>
@@ -6955,7 +6979,7 @@
         <v>7</v>
       </c>
       <c r="H89" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="I89">
         <v>-1</v>
@@ -7005,25 +7029,25 @@
         <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="D90" t="s">
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F90">
         <v>1</v>
       </c>
       <c r="H90" t="s">
-        <v>252</v>
+        <v>266</v>
       </c>
       <c r="I90">
         <v>-1</v>
       </c>
       <c r="J90" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K90">
         <v>3.5</v>
@@ -7067,13 +7091,13 @@
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>177</v>
+        <v>187</v>
       </c>
       <c r="D91" t="s">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -7082,13 +7106,13 @@
         <v>12</v>
       </c>
       <c r="H91" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I91">
         <v>-1</v>
       </c>
       <c r="J91" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="K91">
         <v>4.5</v>
@@ -7132,13 +7156,13 @@
         <v>90</v>
       </c>
       <c r="C92" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D92" t="s">
         <v>1</v>
       </c>
-      <c r="E92" t="s">
-        <v>179</v>
+      <c r="E92">
+        <v>-1</v>
       </c>
       <c r="F92">
         <v>2</v>
@@ -7147,13 +7171,13 @@
         <v>19</v>
       </c>
       <c r="H92" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I92">
         <v>-1</v>
       </c>
       <c r="J92" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K92">
         <v>-1</v>
@@ -7197,13 +7221,13 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="D93" t="s">
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>131</v>
+        <v>142</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -7212,7 +7236,7 @@
         <v>6</v>
       </c>
       <c r="H93" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="I93">
         <v>-1</v>
@@ -7262,13 +7286,13 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
       <c r="D94" t="s">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -7277,7 +7301,7 @@
         <v>6</v>
       </c>
       <c r="H94" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="I94">
         <v>-1</v>
@@ -7327,7 +7351,7 @@
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="D95" t="s">
         <v>1</v>
@@ -7342,13 +7366,13 @@
         <v>7</v>
       </c>
       <c r="H95" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="I95">
         <v>-1</v>
       </c>
       <c r="J95" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K95">
         <v>3.5</v>
@@ -7392,13 +7416,13 @@
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="D96" t="s">
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F96">
         <v>2</v>
@@ -7407,13 +7431,13 @@
         <v>12</v>
       </c>
       <c r="H96" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I96">
         <v>-1</v>
       </c>
       <c r="J96" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K96">
         <v>-1</v>
@@ -7457,13 +7481,13 @@
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="D97" t="s">
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -7472,13 +7496,13 @@
         <v>7</v>
       </c>
       <c r="H97" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="I97">
         <v>-1</v>
       </c>
       <c r="J97" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K97">
         <v>4</v>
@@ -7522,13 +7546,13 @@
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="D98" t="s">
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -7537,13 +7561,13 @@
         <v>12</v>
       </c>
       <c r="H98" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I98">
         <v>-1</v>
       </c>
       <c r="J98" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="K98">
         <v>2.5</v>
@@ -7587,13 +7611,13 @@
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="D99" t="s">
         <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -7602,7 +7626,7 @@
         <v>2</v>
       </c>
       <c r="H99" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="I99">
         <v>-1</v>
@@ -7652,7 +7676,7 @@
         <v>98</v>
       </c>
       <c r="C100" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D100" t="s">
         <v>1</v>
@@ -7667,13 +7691,13 @@
         <v>5</v>
       </c>
       <c r="H100" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I100">
         <v>-1</v>
       </c>
       <c r="J100" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K100">
         <v>-1</v>
@@ -7717,13 +7741,13 @@
         <v>99</v>
       </c>
       <c r="C101" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="D101" t="s">
         <v>1</v>
       </c>
       <c r="E101" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -7732,13 +7756,13 @@
         <v>6</v>
       </c>
       <c r="H101" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="I101">
         <v>-1</v>
       </c>
       <c r="J101" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K101">
         <v>1</v>
@@ -7782,13 +7806,13 @@
         <v>100</v>
       </c>
       <c r="C102" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D102" t="s">
         <v>1</v>
       </c>
-      <c r="E102" t="s">
-        <v>179</v>
+      <c r="E102">
+        <v>-1</v>
       </c>
       <c r="F102">
         <v>3</v>
@@ -7797,13 +7821,13 @@
         <v>20</v>
       </c>
       <c r="H102" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I102">
         <v>-1</v>
       </c>
       <c r="J102" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K102">
         <v>-1</v>
@@ -7847,13 +7871,13 @@
         <v>101</v>
       </c>
       <c r="C103" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="D103" t="s">
         <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F103">
         <v>2</v>
@@ -7862,13 +7886,13 @@
         <v>12</v>
       </c>
       <c r="H103" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I103">
         <v>-1</v>
       </c>
       <c r="J103" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="K103">
         <v>-1</v>
@@ -7912,13 +7936,13 @@
         <v>102</v>
       </c>
       <c r="C104" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="D104" t="s">
         <v>1</v>
       </c>
       <c r="E104" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -7927,13 +7951,13 @@
         <v>6</v>
       </c>
       <c r="H104" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="I104">
         <v>-1</v>
       </c>
       <c r="J104" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K104">
         <v>3</v>
@@ -7977,13 +8001,13 @@
         <v>103</v>
       </c>
       <c r="C105" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="D105" t="s">
         <v>1</v>
       </c>
       <c r="E105" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="F105">
         <v>2</v>
@@ -7992,13 +8016,13 @@
         <v>5</v>
       </c>
       <c r="H105" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I105">
         <v>-1</v>
       </c>
       <c r="J105" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K105">
         <v>-1</v>
@@ -8042,13 +8066,13 @@
         <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="D106" t="s">
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -8057,13 +8081,13 @@
         <v>7</v>
       </c>
       <c r="H106" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="I106">
         <v>-1</v>
       </c>
       <c r="J106" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K106">
         <v>3</v>
@@ -8107,13 +8131,13 @@
         <v>105</v>
       </c>
       <c r="C107" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="D107" t="s">
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -8122,13 +8146,13 @@
         <v>7</v>
       </c>
       <c r="H107" t="s">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c r="I107">
         <v>-1</v>
       </c>
       <c r="J107" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K107">
         <v>3</v>
@@ -8172,7 +8196,7 @@
         <v>106</v>
       </c>
       <c r="C108" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="D108" t="s">
         <v>1</v>
@@ -8187,13 +8211,13 @@
         <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="I108">
         <v>-1</v>
       </c>
       <c r="J108" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="K108">
         <v>-1</v>
@@ -8237,13 +8261,13 @@
         <v>107</v>
       </c>
       <c r="C109" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="D109" t="s">
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F109">
         <v>2</v>
@@ -8252,13 +8276,13 @@
         <v>5</v>
       </c>
       <c r="H109" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I109">
         <v>-1</v>
       </c>
       <c r="J109" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K109">
         <v>-1</v>
@@ -8302,7 +8326,7 @@
         <v>108</v>
       </c>
       <c r="C110" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D110" t="s">
         <v>1</v>
@@ -8317,7 +8341,7 @@
         <v>9</v>
       </c>
       <c r="H110" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I110">
         <v>-1</v>
@@ -8367,13 +8391,13 @@
         <v>109</v>
       </c>
       <c r="C111" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D111" t="s">
         <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F111">
         <v>2</v>
@@ -8382,7 +8406,7 @@
         <v>9</v>
       </c>
       <c r="H111" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I111">
         <v>-1</v>
@@ -8432,13 +8456,13 @@
         <v>110</v>
       </c>
       <c r="C112" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D112" t="s">
         <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="F112">
         <v>2</v>
@@ -8447,7 +8471,7 @@
         <v>9</v>
       </c>
       <c r="H112" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I112">
         <v>-1</v>
@@ -8497,13 +8521,13 @@
         <v>111</v>
       </c>
       <c r="C113" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="D113" t="s">
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F113">
         <v>2</v>
@@ -8512,7 +8536,7 @@
         <v>9</v>
       </c>
       <c r="H113" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I113">
         <v>-1</v>
@@ -8562,13 +8586,13 @@
         <v>112</v>
       </c>
       <c r="C114" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="D114" t="s">
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F114">
         <v>2</v>
@@ -8577,13 +8601,13 @@
         <v>8</v>
       </c>
       <c r="H114" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I114">
         <v>-1</v>
       </c>
       <c r="J114" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="K114">
         <v>-1</v>
@@ -8627,13 +8651,13 @@
         <v>113</v>
       </c>
       <c r="C115" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="D115" t="s">
         <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -8642,7 +8666,7 @@
         <v>6</v>
       </c>
       <c r="H115" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I115">
         <v>-1</v>
@@ -8692,13 +8716,13 @@
         <v>114</v>
       </c>
       <c r="C116" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="D116" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E116" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="F116">
         <v>2</v>
@@ -8707,13 +8731,13 @@
         <v>5</v>
       </c>
       <c r="H116" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="I116">
         <v>-1</v>
       </c>
       <c r="J116" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K116">
         <v>-1</v>
@@ -8757,13 +8781,13 @@
         <v>115</v>
       </c>
       <c r="C117" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="D117" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E117" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F117">
         <v>2</v>
@@ -8772,13 +8796,13 @@
         <v>11</v>
       </c>
       <c r="H117" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I117">
         <v>-1</v>
       </c>
       <c r="J117" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K117">
         <v>-1</v>
@@ -8822,13 +8846,13 @@
         <v>116</v>
       </c>
       <c r="C118" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="D118" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E118" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="F118">
         <v>2</v>
@@ -8837,13 +8861,13 @@
         <v>11</v>
       </c>
       <c r="H118" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I118">
         <v>-1</v>
       </c>
       <c r="J118" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K118">
         <v>-1</v>
@@ -8887,13 +8911,13 @@
         <v>117</v>
       </c>
       <c r="C119" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D119" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E119" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -8902,13 +8926,13 @@
         <v>21</v>
       </c>
       <c r="H119" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I119">
         <v>-1</v>
       </c>
       <c r="J119" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K119">
         <v>1</v>
@@ -8952,13 +8976,13 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>136</v>
+        <v>147</v>
       </c>
       <c r="D120" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E120" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -8967,13 +8991,13 @@
         <v>21</v>
       </c>
       <c r="H120" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I120">
         <v>-1</v>
       </c>
       <c r="J120" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K120">
         <v>1</v>
@@ -9017,13 +9041,13 @@
         <v>119</v>
       </c>
       <c r="C121" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D121" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E121" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="F121">
         <v>2</v>
@@ -9032,7 +9056,7 @@
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="I121">
         <v>-1</v>
@@ -9082,13 +9106,13 @@
         <v>120</v>
       </c>
       <c r="C122" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="D122" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E122" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -9097,13 +9121,13 @@
         <v>12</v>
       </c>
       <c r="H122" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I122">
         <v>-1</v>
       </c>
       <c r="J122" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="K122">
         <v>4</v>
@@ -9147,13 +9171,13 @@
         <v>121</v>
       </c>
       <c r="C123" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D123" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E123" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="F123">
         <v>1</v>
@@ -9162,13 +9186,13 @@
         <v>6</v>
       </c>
       <c r="H123" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I123">
         <v>-1</v>
       </c>
       <c r="J123" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="K123">
         <v>3</v>
@@ -9212,13 +9236,13 @@
         <v>122</v>
       </c>
       <c r="C124" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="D124" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E124" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F124">
         <v>1</v>
@@ -9227,13 +9251,13 @@
         <v>2</v>
       </c>
       <c r="H124" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="I124">
         <v>-1</v>
       </c>
       <c r="J124" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K124">
         <v>3</v>
@@ -9277,13 +9301,13 @@
         <v>123</v>
       </c>
       <c r="C125" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="D125" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E125" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="F125">
         <v>1</v>
@@ -9292,7 +9316,7 @@
         <v>6</v>
       </c>
       <c r="H125" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="I125">
         <v>-1</v>
@@ -9342,13 +9366,13 @@
         <v>124</v>
       </c>
       <c r="C126" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
       <c r="D126" t="s">
-        <v>80</v>
-      </c>
-      <c r="E126" t="s">
-        <v>179</v>
+        <v>87</v>
+      </c>
+      <c r="E126">
+        <v>-1</v>
       </c>
       <c r="F126">
         <v>2</v>
@@ -9357,13 +9381,13 @@
         <v>19</v>
       </c>
       <c r="H126" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I126">
         <v>-1</v>
       </c>
       <c r="J126" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K126">
         <v>-1</v>
@@ -9407,13 +9431,13 @@
         <v>125</v>
       </c>
       <c r="C127" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="D127" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E127" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="F127">
         <v>1</v>
@@ -9422,13 +9446,13 @@
         <v>6</v>
       </c>
       <c r="H127" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="I127">
         <v>-1</v>
       </c>
       <c r="J127" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="K127">
         <v>4.5</v>
@@ -9472,13 +9496,13 @@
         <v>126</v>
       </c>
       <c r="C128" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D128" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E128" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="F128">
         <v>2</v>
@@ -9487,13 +9511,13 @@
         <v>5</v>
       </c>
       <c r="H128" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I128">
         <v>-1</v>
       </c>
       <c r="J128" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K128">
         <v>-1</v>
@@ -9537,13 +9561,13 @@
         <v>127</v>
       </c>
       <c r="C129" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="D129" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E129" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F129">
         <v>2</v>
@@ -9552,13 +9576,13 @@
         <v>5</v>
       </c>
       <c r="H129" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I129">
         <v>-1</v>
       </c>
       <c r="J129" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K129">
         <v>-1</v>
@@ -9602,13 +9626,13 @@
         <v>128</v>
       </c>
       <c r="C130" t="s">
+        <v>221</v>
+      </c>
+      <c r="D130" t="s">
+        <v>87</v>
+      </c>
+      <c r="E130" t="s">
         <v>212</v>
-      </c>
-      <c r="D130" t="s">
-        <v>80</v>
-      </c>
-      <c r="E130" t="s">
-        <v>203</v>
       </c>
       <c r="F130">
         <v>2</v>
@@ -9617,13 +9641,13 @@
         <v>15</v>
       </c>
       <c r="H130" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="I130">
         <v>-1</v>
       </c>
       <c r="J130" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K130">
         <v>-1</v>
@@ -9667,28 +9691,28 @@
         <v>129</v>
       </c>
       <c r="C131" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D131" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E131" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="F131">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G131">
         <v>6</v>
       </c>
       <c r="H131" t="s">
-        <v>138</v>
+        <v>149</v>
       </c>
       <c r="I131">
         <v>-1</v>
       </c>
       <c r="J131" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K131">
         <v>-1</v>
@@ -9732,13 +9756,13 @@
         <v>130</v>
       </c>
       <c r="C132" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D132" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E132" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="F132">
         <v>2</v>
@@ -9747,13 +9771,13 @@
         <v>5</v>
       </c>
       <c r="H132" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I132">
         <v>-1</v>
       </c>
       <c r="J132" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K132">
         <v>-1</v>
@@ -9797,13 +9821,13 @@
         <v>131</v>
       </c>
       <c r="C133" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D133" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E133" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="F133">
         <v>2</v>
@@ -9812,13 +9836,13 @@
         <v>5</v>
       </c>
       <c r="H133" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="I133">
         <v>-1</v>
       </c>
       <c r="J133" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K133">
         <v>-1</v>
@@ -9862,13 +9886,13 @@
         <v>132</v>
       </c>
       <c r="C134" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="D134" t="s">
-        <v>80</v>
-      </c>
-      <c r="E134" t="s">
-        <v>179</v>
+        <v>87</v>
+      </c>
+      <c r="E134">
+        <v>-1</v>
       </c>
       <c r="F134">
         <v>3</v>
@@ -9877,13 +9901,13 @@
         <v>20</v>
       </c>
       <c r="H134" t="s">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="I134">
         <v>-1</v>
       </c>
       <c r="J134" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="K134">
         <v>-1</v>
@@ -9927,13 +9951,13 @@
         <v>133</v>
       </c>
       <c r="C135" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="D135" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E135" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="F135">
         <v>1</v>
@@ -9942,13 +9966,13 @@
         <v>6</v>
       </c>
       <c r="H135" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="I135">
         <v>-1</v>
       </c>
       <c r="J135" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K135">
         <v>3</v>
@@ -9992,13 +10016,13 @@
         <v>134</v>
       </c>
       <c r="C136" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D136" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E136" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -10007,13 +10031,13 @@
         <v>12</v>
       </c>
       <c r="H136" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I136">
         <v>-1</v>
       </c>
       <c r="J136" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="K136">
         <v>3.5</v>
@@ -10057,13 +10081,13 @@
         <v>135</v>
       </c>
       <c r="C137" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D137" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E137" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="F137">
         <v>3</v>
@@ -10072,13 +10096,13 @@
         <v>14</v>
       </c>
       <c r="H137" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="I137">
         <v>-1</v>
       </c>
       <c r="J137" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="K137">
         <v>-1</v>
@@ -10122,13 +10146,13 @@
         <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="D138" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="E138" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="F138">
         <v>2</v>
@@ -10137,13 +10161,13 @@
         <v>8</v>
       </c>
       <c r="H138" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="I138">
         <v>-1</v>
       </c>
       <c r="J138" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="K138">
         <v>-1</v>
@@ -10446,12 +10470,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005FB20A7F2BB1C9418E64F56CA75CF205" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="42ad68925ae8d2a9974bfdc8ea9fefb3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c3d19cc5-3095-4a61-8dd9-9be2b9ec17d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5d68606ac50bf45f4cbba1ccb686340" ns2:_="">
     <xsd:import namespace="c3d19cc5-3095-4a61-8dd9-9be2b9ec17d3"/>
@@ -10583,7 +10601,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -10592,23 +10610,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4362AE6-C2B0-470E-BFFD-18B240FA2FA7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c3d19cc5-3095-4a61-8dd9-9be2b9ec17d3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06EC835C-3161-4414-8CE1-2482AD09E09C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10626,10 +10634,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC3DE6C5-55E9-4C9E-BBC9-8709C3838B15}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4362AE6-C2B0-470E-BFFD-18B240FA2FA7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c3d19cc5-3095-4a61-8dd9-9be2b9ec17d3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Nearly fully functional. Just the actual brute force algorithm left.
</commit_message>
<xml_diff>
--- a/placeAttributes.xlsx
+++ b/placeAttributes.xlsx
@@ -1210,15 +1210,15 @@
   <dimension ref="A1:U203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D62" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="F75" sqref="F75"/>
+      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.140625" bestFit="1" customWidth="1"/>
@@ -10602,18 +10602,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10635,14 +10635,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC3DE6C5-55E9-4C9E-BBC9-8709C3838B15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4362AE6-C2B0-470E-BFFD-18B240FA2FA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -10656,4 +10648,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC3DE6C5-55E9-4C9E-BBC9-8709C3838B15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
most things functional. But when bob clicks Asian it sends him to an Italian restuarant...
</commit_message>
<xml_diff>
--- a/placeAttributes.xlsx
+++ b/placeAttributes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -104,9 +104,6 @@
     <t>7:30 - 20:00</t>
   </si>
   <si>
-    <t>CRÚ - Food &amp; Wine Bar</t>
-  </si>
-  <si>
     <t>6:00 - 22:00</t>
   </si>
   <si>
@@ -849,12 +846,15 @@
   </si>
   <si>
     <t>D30</t>
+  </si>
+  <si>
+    <t>CRU - Food &amp; Wine Bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1210,10 +1210,10 @@
   <dimension ref="A1:U203"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
-      <selection pane="bottomRight" activeCell="G34" sqref="G34"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1241,64 +1241,64 @@
   <sheetData>
     <row r="1" spans="1:21" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>258</v>
-      </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>242</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="J1" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="K1" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="L1" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="K1" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="O1" s="5" t="s">
+      <c r="P1" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="T1" s="5" t="s">
+      <c r="U1" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="U1" s="8" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1392,7 +1392,7 @@
         <v>-1</v>
       </c>
       <c r="I3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J3" t="s">
         <v>7</v>
@@ -1457,7 +1457,7 @@
         <v>-1</v>
       </c>
       <c r="I4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J4" t="s">
         <v>10</v>
@@ -1782,7 +1782,7 @@
         <v>-1</v>
       </c>
       <c r="I9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J9" t="s">
         <v>24</v>
@@ -1829,7 +1829,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>273</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
@@ -1847,10 +1847,10 @@
         <v>-1</v>
       </c>
       <c r="I10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K10">
         <v>3.5</v>
@@ -1894,13 +1894,13 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -1912,7 +1912,7 @@
         <v>-1</v>
       </c>
       <c r="I11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" t="s">
         <v>7</v>
@@ -1959,13 +1959,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
         <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1977,10 +1977,10 @@
         <v>-1</v>
       </c>
       <c r="I12" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K12">
         <v>3</v>
@@ -2024,13 +2024,13 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
         <v>33</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>34</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -2042,7 +2042,7 @@
         <v>-1</v>
       </c>
       <c r="I13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J13" t="s">
         <v>7</v>
@@ -2089,7 +2089,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
@@ -2107,10 +2107,10 @@
         <v>-1</v>
       </c>
       <c r="I14" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14">
         <v>2.5</v>
@@ -2154,7 +2154,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
@@ -2172,10 +2172,10 @@
         <v>-1</v>
       </c>
       <c r="I15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s">
         <v>39</v>
-      </c>
-      <c r="J15" t="s">
-        <v>40</v>
       </c>
       <c r="K15">
         <v>2.5</v>
@@ -2219,13 +2219,13 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
         <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>42</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2237,10 +2237,10 @@
         <v>-1</v>
       </c>
       <c r="I16" t="s">
+        <v>42</v>
+      </c>
+      <c r="J16" t="s">
         <v>43</v>
-      </c>
-      <c r="J16" t="s">
-        <v>44</v>
       </c>
       <c r="K16">
         <v>4</v>
@@ -2284,13 +2284,13 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
         <v>45</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" t="s">
-        <v>46</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -2302,10 +2302,10 @@
         <v>-1</v>
       </c>
       <c r="I17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K17">
         <v>4</v>
@@ -2349,7 +2349,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
@@ -2367,10 +2367,10 @@
         <v>-1</v>
       </c>
       <c r="I18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" t="s">
         <v>49</v>
-      </c>
-      <c r="J18" t="s">
-        <v>50</v>
       </c>
       <c r="K18">
         <v>2.5</v>
@@ -2414,14 +2414,14 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
         <v>51</v>
       </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19" t="s">
-        <v>52</v>
-      </c>
       <c r="F19">
         <v>1</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>-1</v>
       </c>
       <c r="I19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J19" t="s">
         <v>7</v>
@@ -2479,13 +2479,13 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
         <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20" t="s">
-        <v>54</v>
       </c>
       <c r="F20">
         <v>1</v>
@@ -2497,10 +2497,10 @@
         <v>-1</v>
       </c>
       <c r="I20" t="s">
+        <v>54</v>
+      </c>
+      <c r="J20" t="s">
         <v>55</v>
-      </c>
-      <c r="J20" t="s">
-        <v>56</v>
       </c>
       <c r="K20">
         <v>3</v>
@@ -2544,28 +2544,28 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>-1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>263</v>
+      </c>
+      <c r="J21" t="s">
         <v>57</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="H21">
-        <v>-1</v>
-      </c>
-      <c r="I21" t="s">
-        <v>264</v>
-      </c>
-      <c r="J21" t="s">
-        <v>58</v>
       </c>
       <c r="K21">
         <v>3</v>
@@ -2609,7 +2609,7 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -2627,7 +2627,7 @@
         <v>-1</v>
       </c>
       <c r="I22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J22" t="s">
         <v>7</v>
@@ -2674,7 +2674,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
@@ -2692,10 +2692,10 @@
         <v>-1</v>
       </c>
       <c r="I23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K23">
         <v>4</v>
@@ -2739,13 +2739,13 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -2757,10 +2757,10 @@
         <v>-1</v>
       </c>
       <c r="I24" t="s">
+        <v>62</v>
+      </c>
+      <c r="J24" t="s">
         <v>63</v>
-      </c>
-      <c r="J24" t="s">
-        <v>64</v>
       </c>
       <c r="K24">
         <v>3</v>
@@ -2804,13 +2804,13 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>65</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>66</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -2822,10 +2822,10 @@
         <v>-1</v>
       </c>
       <c r="I25" t="s">
+        <v>66</v>
+      </c>
+      <c r="J25" t="s">
         <v>67</v>
-      </c>
-      <c r="J25" t="s">
-        <v>68</v>
       </c>
       <c r="K25">
         <v>3</v>
@@ -2869,13 +2869,13 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>69</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>70</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -2887,10 +2887,10 @@
         <v>-1</v>
       </c>
       <c r="I26" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K26">
         <v>3</v>
@@ -2934,7 +2934,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
@@ -2952,10 +2952,10 @@
         <v>-1</v>
       </c>
       <c r="I27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" t="s">
         <v>73</v>
-      </c>
-      <c r="J27" t="s">
-        <v>74</v>
       </c>
       <c r="K27">
         <v>2</v>
@@ -2999,28 +2999,28 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>-1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>263</v>
+      </c>
+      <c r="J28" t="s">
         <v>75</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-      <c r="G28">
-        <v>2</v>
-      </c>
-      <c r="H28">
-        <v>-1</v>
-      </c>
-      <c r="I28" t="s">
-        <v>264</v>
-      </c>
-      <c r="J28" t="s">
-        <v>76</v>
       </c>
       <c r="K28">
         <v>2.5</v>
@@ -3064,28 +3064,28 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>195</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>-1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>263</v>
+      </c>
+      <c r="J29" t="s">
         <v>75</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>196</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="G29">
-        <v>2</v>
-      </c>
-      <c r="H29">
-        <v>-1</v>
-      </c>
-      <c r="I29" t="s">
-        <v>264</v>
-      </c>
-      <c r="J29" t="s">
-        <v>76</v>
       </c>
       <c r="K29">
         <v>2.5</v>
@@ -3129,28 +3129,28 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>272</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>-1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>263</v>
+      </c>
+      <c r="J30" t="s">
         <v>75</v>
-      </c>
-      <c r="D30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>273</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30">
-        <v>2</v>
-      </c>
-      <c r="H30">
-        <v>-1</v>
-      </c>
-      <c r="I30" t="s">
-        <v>264</v>
-      </c>
-      <c r="J30" t="s">
-        <v>76</v>
       </c>
       <c r="K30">
         <v>2.5</v>
@@ -3194,7 +3194,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
@@ -3212,10 +3212,10 @@
         <v>-1</v>
       </c>
       <c r="I31" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K31">
         <v>2.5</v>
@@ -3259,13 +3259,13 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F32">
         <v>1</v>
@@ -3277,10 +3277,10 @@
         <v>-1</v>
       </c>
       <c r="I32" t="s">
+        <v>78</v>
+      </c>
+      <c r="J32" t="s">
         <v>79</v>
-      </c>
-      <c r="J32" t="s">
-        <v>80</v>
       </c>
       <c r="K32">
         <v>3.5</v>
@@ -3324,13 +3324,13 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
         <v>81</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>82</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -3342,10 +3342,10 @@
         <v>-1</v>
       </c>
       <c r="I33" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K33">
         <v>3.5</v>
@@ -3389,7 +3389,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -3407,7 +3407,7 @@
         <v>-1</v>
       </c>
       <c r="I34" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J34" t="s">
         <v>7</v>
@@ -3454,13 +3454,13 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" t="s">
         <v>86</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>87</v>
-      </c>
-      <c r="E35" t="s">
-        <v>88</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -3472,10 +3472,10 @@
         <v>-1</v>
       </c>
       <c r="I35" t="s">
+        <v>88</v>
+      </c>
+      <c r="J35" t="s">
         <v>89</v>
-      </c>
-      <c r="J35" t="s">
-        <v>90</v>
       </c>
       <c r="K35">
         <v>1.5</v>
@@ -3519,13 +3519,13 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D36" t="s">
+        <v>86</v>
+      </c>
+      <c r="E36" t="s">
         <v>91</v>
-      </c>
-      <c r="D36" t="s">
-        <v>87</v>
-      </c>
-      <c r="E36" t="s">
-        <v>92</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -3537,10 +3537,10 @@
         <v>-1</v>
       </c>
       <c r="I36" t="s">
+        <v>92</v>
+      </c>
+      <c r="J36" t="s">
         <v>93</v>
-      </c>
-      <c r="J36" t="s">
-        <v>94</v>
       </c>
       <c r="K36">
         <v>3.5</v>
@@ -3584,13 +3584,13 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" t="s">
+        <v>86</v>
+      </c>
+      <c r="E37" t="s">
         <v>95</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" t="s">
-        <v>96</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -3602,7 +3602,7 @@
         <v>-1</v>
       </c>
       <c r="I37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J37" t="s">
         <v>7</v>
@@ -3649,28 +3649,28 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" t="s">
+        <v>86</v>
+      </c>
+      <c r="E38" t="s">
         <v>98</v>
       </c>
-      <c r="D38" t="s">
-        <v>87</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>-1</v>
+      </c>
+      <c r="I38" t="s">
+        <v>260</v>
+      </c>
+      <c r="J38" t="s">
         <v>99</v>
-      </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-      <c r="G38">
-        <v>2</v>
-      </c>
-      <c r="H38">
-        <v>-1</v>
-      </c>
-      <c r="I38" t="s">
-        <v>261</v>
-      </c>
-      <c r="J38" t="s">
-        <v>100</v>
       </c>
       <c r="K38">
         <v>4</v>
@@ -3714,13 +3714,13 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="E39" t="s">
         <v>87</v>
-      </c>
-      <c r="E39" t="s">
-        <v>88</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -3732,7 +3732,7 @@
         <v>-1</v>
       </c>
       <c r="I39" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J39" t="s">
         <v>10</v>
@@ -3779,13 +3779,13 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
+        <v>101</v>
+      </c>
+      <c r="D40" t="s">
+        <v>86</v>
+      </c>
+      <c r="E40" t="s">
         <v>102</v>
-      </c>
-      <c r="D40" t="s">
-        <v>87</v>
-      </c>
-      <c r="E40" t="s">
-        <v>103</v>
       </c>
       <c r="F40">
         <v>1</v>
@@ -3797,10 +3797,10 @@
         <v>-1</v>
       </c>
       <c r="I40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J40" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K40">
         <v>3</v>
@@ -3844,13 +3844,13 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -3862,10 +3862,10 @@
         <v>-1</v>
       </c>
       <c r="I41" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K41">
         <v>2.5</v>
@@ -3909,13 +3909,13 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -3927,7 +3927,7 @@
         <v>-1</v>
       </c>
       <c r="I42" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J42" t="s">
         <v>7</v>
@@ -3974,28 +3974,28 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" t="s">
+        <v>86</v>
+      </c>
+      <c r="E43" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>-1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>268</v>
+      </c>
+      <c r="J43" t="s">
         <v>105</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" t="s">
-        <v>96</v>
-      </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-      <c r="G43">
-        <v>2</v>
-      </c>
-      <c r="H43">
-        <v>-1</v>
-      </c>
-      <c r="I43" t="s">
-        <v>269</v>
-      </c>
-      <c r="J43" t="s">
-        <v>106</v>
       </c>
       <c r="K43">
         <v>3</v>
@@ -4039,13 +4039,13 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
+        <v>106</v>
+      </c>
+      <c r="D44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E44" t="s">
         <v>107</v>
-      </c>
-      <c r="D44" t="s">
-        <v>87</v>
-      </c>
-      <c r="E44" t="s">
-        <v>108</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -4057,10 +4057,10 @@
         <v>-1</v>
       </c>
       <c r="I44" t="s">
+        <v>108</v>
+      </c>
+      <c r="J44" t="s">
         <v>109</v>
-      </c>
-      <c r="J44" t="s">
-        <v>110</v>
       </c>
       <c r="K44">
         <v>2</v>
@@ -4104,28 +4104,28 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
+        <v>110</v>
+      </c>
+      <c r="D45" t="s">
+        <v>86</v>
+      </c>
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+      <c r="G45">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>-1</v>
+      </c>
+      <c r="I45" t="s">
+        <v>263</v>
+      </c>
+      <c r="J45" t="s">
         <v>111</v>
-      </c>
-      <c r="D45" t="s">
-        <v>87</v>
-      </c>
-      <c r="E45" t="s">
-        <v>92</v>
-      </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-      <c r="G45">
-        <v>2</v>
-      </c>
-      <c r="H45">
-        <v>-1</v>
-      </c>
-      <c r="I45" t="s">
-        <v>264</v>
-      </c>
-      <c r="J45" t="s">
-        <v>112</v>
       </c>
       <c r="K45">
         <v>2.5</v>
@@ -4169,13 +4169,13 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
+        <v>112</v>
+      </c>
+      <c r="D46" t="s">
+        <v>86</v>
+      </c>
+      <c r="E46" t="s">
         <v>113</v>
-      </c>
-      <c r="D46" t="s">
-        <v>87</v>
-      </c>
-      <c r="E46" t="s">
-        <v>114</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -4187,10 +4187,10 @@
         <v>-1</v>
       </c>
       <c r="I46" t="s">
+        <v>114</v>
+      </c>
+      <c r="J46" t="s">
         <v>115</v>
-      </c>
-      <c r="J46" t="s">
-        <v>116</v>
       </c>
       <c r="K46">
         <v>3.5</v>
@@ -4234,14 +4234,14 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
+        <v>116</v>
+      </c>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+      <c r="E47" t="s">
         <v>117</v>
       </c>
-      <c r="D47" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" t="s">
-        <v>118</v>
-      </c>
       <c r="F47">
         <v>1</v>
       </c>
@@ -4252,7 +4252,7 @@
         <v>-1</v>
       </c>
       <c r="I47" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J47" t="s">
         <v>7</v>
@@ -4299,13 +4299,13 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D48" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -4317,10 +4317,10 @@
         <v>-1</v>
       </c>
       <c r="I48" t="s">
+        <v>119</v>
+      </c>
+      <c r="J48" t="s">
         <v>120</v>
-      </c>
-      <c r="J48" t="s">
-        <v>121</v>
       </c>
       <c r="K48">
         <v>2</v>
@@ -4364,13 +4364,13 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -4382,10 +4382,10 @@
         <v>-1</v>
       </c>
       <c r="I49" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J49" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="K49">
         <v>3.5</v>
@@ -4429,28 +4429,28 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" t="s">
+        <v>86</v>
+      </c>
+      <c r="E50" t="s">
+        <v>123</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>-1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>263</v>
+      </c>
+      <c r="J50" t="s">
         <v>75</v>
-      </c>
-      <c r="D50" t="s">
-        <v>87</v>
-      </c>
-      <c r="E50" t="s">
-        <v>124</v>
-      </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-      <c r="G50">
-        <v>2</v>
-      </c>
-      <c r="H50">
-        <v>-1</v>
-      </c>
-      <c r="I50" t="s">
-        <v>264</v>
-      </c>
-      <c r="J50" t="s">
-        <v>76</v>
       </c>
       <c r="K50">
         <v>2.5</v>
@@ -4494,28 +4494,28 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51" t="s">
+        <v>86</v>
+      </c>
+      <c r="E51" t="s">
+        <v>102</v>
+      </c>
+      <c r="F51">
+        <v>1</v>
+      </c>
+      <c r="G51">
+        <v>2</v>
+      </c>
+      <c r="H51">
+        <v>-1</v>
+      </c>
+      <c r="I51" t="s">
+        <v>263</v>
+      </c>
+      <c r="J51" t="s">
         <v>75</v>
-      </c>
-      <c r="D51" t="s">
-        <v>87</v>
-      </c>
-      <c r="E51" t="s">
-        <v>103</v>
-      </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-      <c r="G51">
-        <v>2</v>
-      </c>
-      <c r="H51">
-        <v>-1</v>
-      </c>
-      <c r="I51" t="s">
-        <v>264</v>
-      </c>
-      <c r="J51" t="s">
-        <v>76</v>
       </c>
       <c r="K51">
         <v>2.5</v>
@@ -4559,13 +4559,13 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D52" t="s">
+        <v>86</v>
+      </c>
+      <c r="E52" t="s">
         <v>125</v>
-      </c>
-      <c r="D52" t="s">
-        <v>87</v>
-      </c>
-      <c r="E52" t="s">
-        <v>126</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -4577,10 +4577,10 @@
         <v>-1</v>
       </c>
       <c r="I52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K52">
         <v>3.5</v>
@@ -4624,13 +4624,13 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
+        <v>127</v>
+      </c>
+      <c r="D53" t="s">
+        <v>86</v>
+      </c>
+      <c r="E53" t="s">
         <v>128</v>
-      </c>
-      <c r="D53" t="s">
-        <v>87</v>
-      </c>
-      <c r="E53" t="s">
-        <v>129</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -4642,10 +4642,10 @@
         <v>-1</v>
       </c>
       <c r="I53" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K53">
         <v>2.5</v>
@@ -4689,13 +4689,13 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D54" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E54" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -4707,7 +4707,7 @@
         <v>-1</v>
       </c>
       <c r="I54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J54" t="s">
         <v>10</v>
@@ -4754,13 +4754,13 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F55">
         <v>2</v>
@@ -4769,13 +4769,13 @@
         <v>5</v>
       </c>
       <c r="H55" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I55">
         <v>-1</v>
       </c>
       <c r="J55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K55">
         <v>-1</v>
@@ -4819,13 +4819,13 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F56">
         <v>2</v>
@@ -4834,13 +4834,13 @@
         <v>12</v>
       </c>
       <c r="H56" t="s">
+        <v>135</v>
+      </c>
+      <c r="I56">
+        <v>-1</v>
+      </c>
+      <c r="J56" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="I56">
-        <v>-1</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="K56">
         <v>-1</v>
@@ -4884,7 +4884,7 @@
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
@@ -4899,13 +4899,13 @@
         <v>11</v>
       </c>
       <c r="H57" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I57">
         <v>-1</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K57">
         <v>-1</v>
@@ -4949,13 +4949,13 @@
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D58" t="s">
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F58">
         <v>3</v>
@@ -4964,13 +4964,13 @@
         <v>11</v>
       </c>
       <c r="H58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I58">
         <v>-1</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K58">
         <v>-1</v>
@@ -5014,13 +5014,13 @@
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F59">
         <v>3</v>
@@ -5029,13 +5029,13 @@
         <v>11</v>
       </c>
       <c r="H59" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I59">
         <v>-1</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K59">
         <v>-1</v>
@@ -5079,13 +5079,13 @@
         <v>58</v>
       </c>
       <c r="C60" t="s">
+        <v>140</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60" t="s">
         <v>141</v>
-      </c>
-      <c r="D60" t="s">
-        <v>1</v>
-      </c>
-      <c r="E60" t="s">
-        <v>142</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -5094,13 +5094,13 @@
         <v>7</v>
       </c>
       <c r="H60" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I60">
         <v>-1</v>
       </c>
       <c r="J60" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K60">
         <v>3</v>
@@ -5144,13 +5144,13 @@
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -5159,13 +5159,13 @@
         <v>7</v>
       </c>
       <c r="H61" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I61">
         <v>-1</v>
       </c>
       <c r="J61" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K61">
         <v>3</v>
@@ -5209,13 +5209,13 @@
         <v>60</v>
       </c>
       <c r="C62" t="s">
+        <v>143</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" t="s">
         <v>144</v>
-      </c>
-      <c r="D62" t="s">
-        <v>1</v>
-      </c>
-      <c r="E62" t="s">
-        <v>145</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -5224,13 +5224,13 @@
         <v>7</v>
       </c>
       <c r="H62" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I62">
         <v>-1</v>
       </c>
       <c r="J62" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K62">
         <v>4.5</v>
@@ -5274,13 +5274,13 @@
         <v>61</v>
       </c>
       <c r="C63" t="s">
+        <v>146</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" t="s">
         <v>147</v>
-      </c>
-      <c r="D63" t="s">
-        <v>1</v>
-      </c>
-      <c r="E63" t="s">
-        <v>148</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -5289,13 +5289,13 @@
         <v>6</v>
       </c>
       <c r="H63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I63">
         <v>-1</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -5339,13 +5339,13 @@
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -5354,13 +5354,13 @@
         <v>6</v>
       </c>
       <c r="H64" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I64">
         <v>-1</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -5404,7 +5404,7 @@
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
@@ -5419,13 +5419,13 @@
         <v>6</v>
       </c>
       <c r="H65" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I65">
         <v>-1</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -5469,13 +5469,13 @@
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F66">
         <v>2</v>
@@ -5484,13 +5484,13 @@
         <v>12</v>
       </c>
       <c r="H66" t="s">
+        <v>135</v>
+      </c>
+      <c r="I66">
+        <v>-1</v>
+      </c>
+      <c r="J66" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="I66">
-        <v>-1</v>
-      </c>
-      <c r="J66" s="3" t="s">
-        <v>137</v>
       </c>
       <c r="K66">
         <v>-1</v>
@@ -5534,13 +5534,13 @@
         <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D67" t="s">
         <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -5549,13 +5549,13 @@
         <v>7</v>
       </c>
       <c r="H67" t="s">
+        <v>152</v>
+      </c>
+      <c r="I67">
+        <v>-1</v>
+      </c>
+      <c r="J67" t="s">
         <v>153</v>
-      </c>
-      <c r="I67">
-        <v>-1</v>
-      </c>
-      <c r="J67" t="s">
-        <v>154</v>
       </c>
       <c r="K67">
         <v>4</v>
@@ -5599,13 +5599,13 @@
         <v>66</v>
       </c>
       <c r="C68" t="s">
+        <v>154</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
         <v>155</v>
-      </c>
-      <c r="D68" t="s">
-        <v>1</v>
-      </c>
-      <c r="E68" t="s">
-        <v>156</v>
       </c>
       <c r="F68">
         <v>2</v>
@@ -5614,7 +5614,7 @@
         <v>5</v>
       </c>
       <c r="H68" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I68">
         <v>-1</v>
@@ -5664,13 +5664,13 @@
         <v>67</v>
       </c>
       <c r="C69" t="s">
+        <v>157</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
         <v>158</v>
-      </c>
-      <c r="D69" t="s">
-        <v>1</v>
-      </c>
-      <c r="E69" t="s">
-        <v>159</v>
       </c>
       <c r="F69">
         <v>2</v>
@@ -5679,7 +5679,7 @@
         <v>9</v>
       </c>
       <c r="H69" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I69">
         <v>-1</v>
@@ -5729,13 +5729,13 @@
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D70" t="s">
         <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F70">
         <v>2</v>
@@ -5744,13 +5744,13 @@
         <v>9</v>
       </c>
       <c r="H70" t="s">
+        <v>160</v>
+      </c>
+      <c r="I70">
+        <v>-1</v>
+      </c>
+      <c r="J70" t="s">
         <v>161</v>
-      </c>
-      <c r="I70">
-        <v>-1</v>
-      </c>
-      <c r="J70" t="s">
-        <v>162</v>
       </c>
       <c r="K70">
         <v>-1</v>
@@ -5794,7 +5794,7 @@
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
@@ -5809,13 +5809,13 @@
         <v>9</v>
       </c>
       <c r="H71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I71">
         <v>-1</v>
       </c>
       <c r="J71" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K71">
         <v>-1</v>
@@ -5859,7 +5859,7 @@
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D72" t="s">
         <v>1</v>
@@ -5874,13 +5874,13 @@
         <v>9</v>
       </c>
       <c r="H72" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I72">
         <v>-1</v>
       </c>
       <c r="J72" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K72">
         <v>-1</v>
@@ -5924,13 +5924,13 @@
         <v>71</v>
       </c>
       <c r="C73" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D73" t="s">
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F73">
         <v>2</v>
@@ -5939,13 +5939,13 @@
         <v>9</v>
       </c>
       <c r="H73" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I73">
         <v>-1</v>
       </c>
       <c r="J73" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K73">
         <v>-1</v>
@@ -5989,13 +5989,13 @@
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F74">
         <v>2</v>
@@ -6004,13 +6004,13 @@
         <v>18</v>
       </c>
       <c r="H74" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I74">
         <v>-1</v>
       </c>
       <c r="J74" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K74">
         <v>-1</v>
@@ -6054,7 +6054,7 @@
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D75" t="s">
         <v>1</v>
@@ -6069,7 +6069,7 @@
         <v>6</v>
       </c>
       <c r="H75" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I75">
         <v>-1</v>
@@ -6119,13 +6119,13 @@
         <v>74</v>
       </c>
       <c r="C76" t="s">
+        <v>168</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
         <v>169</v>
-      </c>
-      <c r="D76" t="s">
-        <v>1</v>
-      </c>
-      <c r="E76" t="s">
-        <v>170</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -6134,7 +6134,7 @@
         <v>7</v>
       </c>
       <c r="H76" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I76">
         <v>-1</v>
@@ -6184,13 +6184,13 @@
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D77" t="s">
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -6199,7 +6199,7 @@
         <v>7</v>
       </c>
       <c r="H77" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I77">
         <v>-1</v>
@@ -6249,28 +6249,28 @@
         <v>76</v>
       </c>
       <c r="C78" t="s">
+        <v>171</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>69</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>2</v>
+      </c>
+      <c r="H78" t="s">
         <v>172</v>
       </c>
-      <c r="D78" t="s">
-        <v>1</v>
-      </c>
-      <c r="E78" t="s">
-        <v>70</v>
-      </c>
-      <c r="F78">
-        <v>1</v>
-      </c>
-      <c r="G78">
-        <v>2</v>
-      </c>
-      <c r="H78" t="s">
-        <v>173</v>
-      </c>
       <c r="I78">
         <v>-1</v>
       </c>
       <c r="J78" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K78">
         <v>4.5</v>
@@ -6314,13 +6314,13 @@
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D79" t="s">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F79">
         <v>1</v>
@@ -6329,13 +6329,13 @@
         <v>7</v>
       </c>
       <c r="H79" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I79">
         <v>-1</v>
       </c>
       <c r="J79" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K79">
         <v>5</v>
@@ -6379,7 +6379,7 @@
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D80" t="s">
         <v>1</v>
@@ -6394,13 +6394,13 @@
         <v>5</v>
       </c>
       <c r="H80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I80">
         <v>-1</v>
       </c>
       <c r="J80" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K80">
         <v>-1</v>
@@ -6444,13 +6444,13 @@
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D81" t="s">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -6459,13 +6459,13 @@
         <v>7</v>
       </c>
       <c r="H81" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I81">
         <v>-1</v>
       </c>
       <c r="J81" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K81">
         <v>3.5</v>
@@ -6509,13 +6509,13 @@
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D82" t="s">
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F82">
         <v>1</v>
@@ -6524,13 +6524,13 @@
         <v>6</v>
       </c>
       <c r="H82" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I82">
         <v>-1</v>
       </c>
       <c r="J82" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K82">
         <v>3</v>
@@ -6574,13 +6574,13 @@
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F83">
         <v>1</v>
@@ -6589,13 +6589,13 @@
         <v>7</v>
       </c>
       <c r="H83" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I83">
         <v>-1</v>
       </c>
       <c r="J83" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K83">
         <v>3.5</v>
@@ -6639,13 +6639,13 @@
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D84" t="s">
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F84">
         <v>1</v>
@@ -6654,13 +6654,13 @@
         <v>7</v>
       </c>
       <c r="H84" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I84">
         <v>-1</v>
       </c>
       <c r="J84" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K84">
         <v>3.5</v>
@@ -6704,7 +6704,7 @@
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D85" t="s">
         <v>1</v>
@@ -6719,13 +6719,13 @@
         <v>7</v>
       </c>
       <c r="H85" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I85">
         <v>-1</v>
       </c>
       <c r="J85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K85">
         <v>3.5</v>
@@ -6769,13 +6769,13 @@
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D86" t="s">
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -6784,7 +6784,7 @@
         <v>6</v>
       </c>
       <c r="H86" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I86">
         <v>-1</v>
@@ -6834,13 +6834,13 @@
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D87" t="s">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -6849,13 +6849,13 @@
         <v>12</v>
       </c>
       <c r="H87" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I87">
         <v>-1</v>
       </c>
       <c r="J87" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K87">
         <v>2.5</v>
@@ -6899,13 +6899,13 @@
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D88" t="s">
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -6914,7 +6914,7 @@
         <v>7</v>
       </c>
       <c r="H88" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I88">
         <v>-1</v>
@@ -6964,7 +6964,7 @@
         <v>87</v>
       </c>
       <c r="C89" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D89" t="s">
         <v>1</v>
@@ -6979,7 +6979,7 @@
         <v>7</v>
       </c>
       <c r="H89" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="I89">
         <v>-1</v>
@@ -7029,25 +7029,25 @@
         <v>88</v>
       </c>
       <c r="C90" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D90" t="s">
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F90">
         <v>1</v>
       </c>
       <c r="H90" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I90">
         <v>-1</v>
       </c>
       <c r="J90" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K90">
         <v>3.5</v>
@@ -7091,13 +7091,13 @@
         <v>89</v>
       </c>
       <c r="C91" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D91" t="s">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -7106,13 +7106,13 @@
         <v>12</v>
       </c>
       <c r="H91" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I91">
         <v>-1</v>
       </c>
       <c r="J91" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K91">
         <v>4.5</v>
@@ -7156,7 +7156,7 @@
         <v>90</v>
       </c>
       <c r="C92" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D92" t="s">
         <v>1</v>
@@ -7171,13 +7171,13 @@
         <v>19</v>
       </c>
       <c r="H92" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I92">
         <v>-1</v>
       </c>
       <c r="J92" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K92">
         <v>-1</v>
@@ -7221,13 +7221,13 @@
         <v>91</v>
       </c>
       <c r="C93" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D93" t="s">
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -7236,7 +7236,7 @@
         <v>6</v>
       </c>
       <c r="H93" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I93">
         <v>-1</v>
@@ -7286,13 +7286,13 @@
         <v>92</v>
       </c>
       <c r="C94" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D94" t="s">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -7301,7 +7301,7 @@
         <v>6</v>
       </c>
       <c r="H94" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I94">
         <v>-1</v>
@@ -7351,7 +7351,7 @@
         <v>93</v>
       </c>
       <c r="C95" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D95" t="s">
         <v>1</v>
@@ -7366,13 +7366,13 @@
         <v>7</v>
       </c>
       <c r="H95" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I95">
         <v>-1</v>
       </c>
       <c r="J95" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K95">
         <v>3.5</v>
@@ -7416,13 +7416,13 @@
         <v>94</v>
       </c>
       <c r="C96" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D96" t="s">
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F96">
         <v>2</v>
@@ -7431,13 +7431,13 @@
         <v>12</v>
       </c>
       <c r="H96" t="s">
+        <v>135</v>
+      </c>
+      <c r="I96">
+        <v>-1</v>
+      </c>
+      <c r="J96" t="s">
         <v>136</v>
-      </c>
-      <c r="I96">
-        <v>-1</v>
-      </c>
-      <c r="J96" t="s">
-        <v>137</v>
       </c>
       <c r="K96">
         <v>-1</v>
@@ -7481,13 +7481,13 @@
         <v>95</v>
       </c>
       <c r="C97" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D97" t="s">
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -7496,13 +7496,13 @@
         <v>7</v>
       </c>
       <c r="H97" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I97">
         <v>-1</v>
       </c>
       <c r="J97" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K97">
         <v>4</v>
@@ -7546,13 +7546,13 @@
         <v>96</v>
       </c>
       <c r="C98" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D98" t="s">
         <v>1</v>
       </c>
       <c r="E98" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -7561,13 +7561,13 @@
         <v>12</v>
       </c>
       <c r="H98" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I98">
         <v>-1</v>
       </c>
       <c r="J98" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K98">
         <v>2.5</v>
@@ -7611,13 +7611,13 @@
         <v>97</v>
       </c>
       <c r="C99" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D99" t="s">
         <v>1</v>
       </c>
       <c r="E99" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F99">
         <v>1</v>
@@ -7626,7 +7626,7 @@
         <v>2</v>
       </c>
       <c r="H99" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I99">
         <v>-1</v>
@@ -7676,7 +7676,7 @@
         <v>98</v>
       </c>
       <c r="C100" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D100" t="s">
         <v>1</v>
@@ -7691,13 +7691,13 @@
         <v>5</v>
       </c>
       <c r="H100" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I100">
         <v>-1</v>
       </c>
       <c r="J100" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K100">
         <v>-1</v>
@@ -7741,13 +7741,13 @@
         <v>99</v>
       </c>
       <c r="C101" t="s">
+        <v>194</v>
+      </c>
+      <c r="D101" t="s">
+        <v>1</v>
+      </c>
+      <c r="E101" t="s">
         <v>195</v>
-      </c>
-      <c r="D101" t="s">
-        <v>1</v>
-      </c>
-      <c r="E101" t="s">
-        <v>196</v>
       </c>
       <c r="F101">
         <v>1</v>
@@ -7756,13 +7756,13 @@
         <v>6</v>
       </c>
       <c r="H101" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I101">
         <v>-1</v>
       </c>
       <c r="J101" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K101">
         <v>1</v>
@@ -7806,7 +7806,7 @@
         <v>100</v>
       </c>
       <c r="C102" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D102" t="s">
         <v>1</v>
@@ -7821,13 +7821,13 @@
         <v>20</v>
       </c>
       <c r="H102" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I102">
         <v>-1</v>
       </c>
       <c r="J102" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K102">
         <v>-1</v>
@@ -7871,13 +7871,13 @@
         <v>101</v>
       </c>
       <c r="C103" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D103" t="s">
         <v>1</v>
       </c>
       <c r="E103" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F103">
         <v>2</v>
@@ -7886,13 +7886,13 @@
         <v>12</v>
       </c>
       <c r="H103" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I103">
         <v>-1</v>
       </c>
       <c r="J103" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K103">
         <v>-1</v>
@@ -7936,13 +7936,13 @@
         <v>102</v>
       </c>
       <c r="C104" t="s">
+        <v>199</v>
+      </c>
+      <c r="D104" t="s">
+        <v>1</v>
+      </c>
+      <c r="E104" t="s">
         <v>200</v>
-      </c>
-      <c r="D104" t="s">
-        <v>1</v>
-      </c>
-      <c r="E104" t="s">
-        <v>201</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -7951,13 +7951,13 @@
         <v>6</v>
       </c>
       <c r="H104" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I104">
         <v>-1</v>
       </c>
       <c r="J104" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K104">
         <v>3</v>
@@ -8001,13 +8001,13 @@
         <v>103</v>
       </c>
       <c r="C105" t="s">
+        <v>201</v>
+      </c>
+      <c r="D105" t="s">
+        <v>1</v>
+      </c>
+      <c r="E105" t="s">
         <v>202</v>
-      </c>
-      <c r="D105" t="s">
-        <v>1</v>
-      </c>
-      <c r="E105" t="s">
-        <v>203</v>
       </c>
       <c r="F105">
         <v>2</v>
@@ -8016,13 +8016,13 @@
         <v>5</v>
       </c>
       <c r="H105" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I105">
         <v>-1</v>
       </c>
       <c r="J105" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K105">
         <v>-1</v>
@@ -8066,13 +8066,13 @@
         <v>104</v>
       </c>
       <c r="C106" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D106" t="s">
         <v>1</v>
       </c>
       <c r="E106" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -8081,13 +8081,13 @@
         <v>7</v>
       </c>
       <c r="H106" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="I106">
         <v>-1</v>
       </c>
       <c r="J106" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K106">
         <v>3</v>
@@ -8131,13 +8131,13 @@
         <v>105</v>
       </c>
       <c r="C107" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D107" t="s">
         <v>1</v>
       </c>
       <c r="E107" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -8146,13 +8146,13 @@
         <v>7</v>
       </c>
       <c r="H107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I107">
         <v>-1</v>
       </c>
       <c r="J107" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K107">
         <v>3</v>
@@ -8196,7 +8196,7 @@
         <v>106</v>
       </c>
       <c r="C108" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D108" t="s">
         <v>1</v>
@@ -8211,13 +8211,13 @@
         <v>12</v>
       </c>
       <c r="H108" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I108">
         <v>-1</v>
       </c>
       <c r="J108" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K108">
         <v>-1</v>
@@ -8261,13 +8261,13 @@
         <v>107</v>
       </c>
       <c r="C109" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D109" t="s">
         <v>1</v>
       </c>
       <c r="E109" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F109">
         <v>2</v>
@@ -8276,13 +8276,13 @@
         <v>5</v>
       </c>
       <c r="H109" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I109">
         <v>-1</v>
       </c>
       <c r="J109" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K109">
         <v>-1</v>
@@ -8326,7 +8326,7 @@
         <v>108</v>
       </c>
       <c r="C110" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D110" t="s">
         <v>1</v>
@@ -8341,7 +8341,7 @@
         <v>9</v>
       </c>
       <c r="H110" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I110">
         <v>-1</v>
@@ -8391,13 +8391,13 @@
         <v>109</v>
       </c>
       <c r="C111" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D111" t="s">
         <v>1</v>
       </c>
       <c r="E111" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F111">
         <v>2</v>
@@ -8406,7 +8406,7 @@
         <v>9</v>
       </c>
       <c r="H111" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I111">
         <v>-1</v>
@@ -8456,13 +8456,13 @@
         <v>110</v>
       </c>
       <c r="C112" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D112" t="s">
         <v>1</v>
       </c>
       <c r="E112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F112">
         <v>2</v>
@@ -8471,7 +8471,7 @@
         <v>9</v>
       </c>
       <c r="H112" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I112">
         <v>-1</v>
@@ -8521,13 +8521,13 @@
         <v>111</v>
       </c>
       <c r="C113" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D113" t="s">
         <v>1</v>
       </c>
       <c r="E113" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F113">
         <v>2</v>
@@ -8536,7 +8536,7 @@
         <v>9</v>
       </c>
       <c r="H113" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I113">
         <v>-1</v>
@@ -8586,13 +8586,13 @@
         <v>112</v>
       </c>
       <c r="C114" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D114" t="s">
         <v>1</v>
       </c>
       <c r="E114" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F114">
         <v>2</v>
@@ -8601,13 +8601,13 @@
         <v>8</v>
       </c>
       <c r="H114" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I114">
         <v>-1</v>
       </c>
       <c r="J114" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K114">
         <v>-1</v>
@@ -8651,13 +8651,13 @@
         <v>113</v>
       </c>
       <c r="C115" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D115" t="s">
         <v>1</v>
       </c>
       <c r="E115" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -8666,7 +8666,7 @@
         <v>6</v>
       </c>
       <c r="H115" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I115">
         <v>-1</v>
@@ -8716,13 +8716,13 @@
         <v>114</v>
       </c>
       <c r="C116" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D116" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E116" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F116">
         <v>2</v>
@@ -8731,13 +8731,13 @@
         <v>5</v>
       </c>
       <c r="H116" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="I116">
         <v>-1</v>
       </c>
       <c r="J116" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K116">
         <v>-1</v>
@@ -8781,13 +8781,13 @@
         <v>115</v>
       </c>
       <c r="C117" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D117" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E117" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F117">
         <v>2</v>
@@ -8796,13 +8796,13 @@
         <v>11</v>
       </c>
       <c r="H117" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I117">
         <v>-1</v>
       </c>
       <c r="J117" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K117">
         <v>-1</v>
@@ -8846,13 +8846,13 @@
         <v>116</v>
       </c>
       <c r="C118" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D118" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E118" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F118">
         <v>2</v>
@@ -8861,13 +8861,13 @@
         <v>11</v>
       </c>
       <c r="H118" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I118">
         <v>-1</v>
       </c>
       <c r="J118" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K118">
         <v>-1</v>
@@ -8911,13 +8911,13 @@
         <v>117</v>
       </c>
       <c r="C119" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D119" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E119" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -8926,13 +8926,13 @@
         <v>21</v>
       </c>
       <c r="H119" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I119">
         <v>-1</v>
       </c>
       <c r="J119" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K119">
         <v>1</v>
@@ -8976,13 +8976,13 @@
         <v>118</v>
       </c>
       <c r="C120" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D120" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E120" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -8991,13 +8991,13 @@
         <v>21</v>
       </c>
       <c r="H120" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I120">
         <v>-1</v>
       </c>
       <c r="J120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K120">
         <v>1</v>
@@ -9041,13 +9041,13 @@
         <v>119</v>
       </c>
       <c r="C121" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D121" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E121" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F121">
         <v>2</v>
@@ -9056,7 +9056,7 @@
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I121">
         <v>-1</v>
@@ -9106,13 +9106,13 @@
         <v>120</v>
       </c>
       <c r="C122" t="s">
+        <v>213</v>
+      </c>
+      <c r="D122" t="s">
+        <v>86</v>
+      </c>
+      <c r="E122" t="s">
         <v>214</v>
-      </c>
-      <c r="D122" t="s">
-        <v>87</v>
-      </c>
-      <c r="E122" t="s">
-        <v>215</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -9121,13 +9121,13 @@
         <v>12</v>
       </c>
       <c r="H122" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I122">
         <v>-1</v>
       </c>
       <c r="J122" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K122">
         <v>4</v>
@@ -9171,13 +9171,13 @@
         <v>121</v>
       </c>
       <c r="C123" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D123" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E123" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F123">
         <v>1</v>
@@ -9186,13 +9186,13 @@
         <v>6</v>
       </c>
       <c r="H123" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I123">
         <v>-1</v>
       </c>
       <c r="J123" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K123">
         <v>3</v>
@@ -9236,13 +9236,13 @@
         <v>122</v>
       </c>
       <c r="C124" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D124" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E124" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F124">
         <v>1</v>
@@ -9251,13 +9251,13 @@
         <v>2</v>
       </c>
       <c r="H124" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I124">
         <v>-1</v>
       </c>
       <c r="J124" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K124">
         <v>3</v>
@@ -9301,13 +9301,13 @@
         <v>123</v>
       </c>
       <c r="C125" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D125" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E125" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F125">
         <v>1</v>
@@ -9316,7 +9316,7 @@
         <v>6</v>
       </c>
       <c r="H125" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I125">
         <v>-1</v>
@@ -9366,10 +9366,10 @@
         <v>124</v>
       </c>
       <c r="C126" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D126" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E126">
         <v>-1</v>
@@ -9381,13 +9381,13 @@
         <v>19</v>
       </c>
       <c r="H126" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I126">
         <v>-1</v>
       </c>
       <c r="J126" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K126">
         <v>-1</v>
@@ -9431,13 +9431,13 @@
         <v>125</v>
       </c>
       <c r="C127" t="s">
+        <v>217</v>
+      </c>
+      <c r="D127" t="s">
+        <v>86</v>
+      </c>
+      <c r="E127" t="s">
         <v>218</v>
-      </c>
-      <c r="D127" t="s">
-        <v>87</v>
-      </c>
-      <c r="E127" t="s">
-        <v>219</v>
       </c>
       <c r="F127">
         <v>1</v>
@@ -9446,13 +9446,13 @@
         <v>6</v>
       </c>
       <c r="H127" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I127">
         <v>-1</v>
       </c>
       <c r="J127" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K127">
         <v>4.5</v>
@@ -9496,13 +9496,13 @@
         <v>126</v>
       </c>
       <c r="C128" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D128" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E128" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F128">
         <v>2</v>
@@ -9511,13 +9511,13 @@
         <v>5</v>
       </c>
       <c r="H128" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I128">
         <v>-1</v>
       </c>
       <c r="J128" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K128">
         <v>-1</v>
@@ -9561,13 +9561,13 @@
         <v>127</v>
       </c>
       <c r="C129" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D129" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E129" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F129">
         <v>2</v>
@@ -9576,13 +9576,13 @@
         <v>5</v>
       </c>
       <c r="H129" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I129">
         <v>-1</v>
       </c>
       <c r="J129" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K129">
         <v>-1</v>
@@ -9626,13 +9626,13 @@
         <v>128</v>
       </c>
       <c r="C130" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D130" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E130" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F130">
         <v>2</v>
@@ -9641,13 +9641,13 @@
         <v>15</v>
       </c>
       <c r="H130" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I130">
         <v>-1</v>
       </c>
       <c r="J130" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K130">
         <v>-1</v>
@@ -9691,13 +9691,13 @@
         <v>129</v>
       </c>
       <c r="C131" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D131" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E131" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F131">
         <v>1</v>
@@ -9706,13 +9706,13 @@
         <v>6</v>
       </c>
       <c r="H131" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I131">
         <v>-1</v>
       </c>
       <c r="J131" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K131">
         <v>-1</v>
@@ -9756,13 +9756,13 @@
         <v>130</v>
       </c>
       <c r="C132" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D132" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E132" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="F132">
         <v>2</v>
@@ -9771,13 +9771,13 @@
         <v>5</v>
       </c>
       <c r="H132" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I132">
         <v>-1</v>
       </c>
       <c r="J132" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K132">
         <v>-1</v>
@@ -9821,13 +9821,13 @@
         <v>131</v>
       </c>
       <c r="C133" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D133" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E133" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F133">
         <v>2</v>
@@ -9836,13 +9836,13 @@
         <v>5</v>
       </c>
       <c r="H133" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I133">
         <v>-1</v>
       </c>
       <c r="J133" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K133">
         <v>-1</v>
@@ -9886,10 +9886,10 @@
         <v>132</v>
       </c>
       <c r="C134" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D134" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E134">
         <v>-1</v>
@@ -9901,13 +9901,13 @@
         <v>20</v>
       </c>
       <c r="H134" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I134">
         <v>-1</v>
       </c>
       <c r="J134" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K134">
         <v>-1</v>
@@ -9951,13 +9951,13 @@
         <v>133</v>
       </c>
       <c r="C135" t="s">
+        <v>223</v>
+      </c>
+      <c r="D135" t="s">
+        <v>86</v>
+      </c>
+      <c r="E135" t="s">
         <v>224</v>
-      </c>
-      <c r="D135" t="s">
-        <v>87</v>
-      </c>
-      <c r="E135" t="s">
-        <v>225</v>
       </c>
       <c r="F135">
         <v>1</v>
@@ -9966,13 +9966,13 @@
         <v>6</v>
       </c>
       <c r="H135" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I135">
         <v>-1</v>
       </c>
       <c r="J135" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K135">
         <v>3</v>
@@ -10016,13 +10016,13 @@
         <v>134</v>
       </c>
       <c r="C136" t="s">
+        <v>226</v>
+      </c>
+      <c r="D136" t="s">
+        <v>86</v>
+      </c>
+      <c r="E136" t="s">
         <v>227</v>
-      </c>
-      <c r="D136" t="s">
-        <v>87</v>
-      </c>
-      <c r="E136" t="s">
-        <v>228</v>
       </c>
       <c r="F136">
         <v>1</v>
@@ -10031,13 +10031,13 @@
         <v>12</v>
       </c>
       <c r="H136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I136">
         <v>-1</v>
       </c>
       <c r="J136" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="K136">
         <v>3.5</v>
@@ -10081,13 +10081,13 @@
         <v>135</v>
       </c>
       <c r="C137" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D137" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E137" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F137">
         <v>3</v>
@@ -10096,13 +10096,13 @@
         <v>14</v>
       </c>
       <c r="H137" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="I137">
         <v>-1</v>
       </c>
       <c r="J137" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="K137">
         <v>-1</v>
@@ -10146,13 +10146,13 @@
         <v>136</v>
       </c>
       <c r="C138" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D138" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E138" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F138">
         <v>2</v>
@@ -10161,13 +10161,13 @@
         <v>8</v>
       </c>
       <c r="H138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I138">
         <v>-1</v>
       </c>
       <c r="J138" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K138">
         <v>-1</v>
@@ -10602,18 +10602,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10635,6 +10635,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC3DE6C5-55E9-4C9E-BBC9-8709C3838B15}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4362AE6-C2B0-470E-BFFD-18B240FA2FA7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -10648,12 +10656,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BC3DE6C5-55E9-4C9E-BBC9-8709C3838B15}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>